<commit_message>
testRoomInitials now passing, needed to not load bad configs.
</commit_message>
<xml_diff>
--- a/ClueBoard/CR_ClueLayoutBadRoom.xlsx
+++ b/ClueBoard/CR_ClueLayoutBadRoom.xlsx
@@ -1239,9 +1239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>